<commit_message>
optimizacion de conteo de horas laborales
</commit_message>
<xml_diff>
--- a/assets/Template.xlsx
+++ b/assets/Template.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Escritorio\Projects\area51-backend\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F28CCE6-CE35-4702-977F-640AA4EA4014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1548" yWindow="2016" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Hoja 2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Hoja 3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Hoja 4" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Hoja 5" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Hoja 6" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Hoja 7" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Hoja 8" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Hoja 9" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="Hoja 10" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="Hoja 11" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="Hoja 12" sheetId="12" r:id="rId15"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Hoja 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Hoja 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Hoja 9" sheetId="9" r:id="rId9"/>
+    <sheet name="Hoja 10" sheetId="10" r:id="rId10"/>
+    <sheet name="Hoja 11" sheetId="11" r:id="rId11"/>
+    <sheet name="Hoja 12" sheetId="12" r:id="rId12"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -69,27 +78,47 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -97,7 +126,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -131,96 +160,76 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -410,95 +419,118 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="A5:E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -506,59 +538,73 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -575,29 +621,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -605,59 +656,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -674,29 +738,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -704,60 +773,73 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -773,29 +855,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -803,59 +890,74 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -872,29 +974,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -902,59 +1009,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -971,29 +1091,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -1001,59 +1126,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1070,29 +1208,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -1100,59 +1243,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1169,29 +1325,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -1199,59 +1360,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1268,29 +1442,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -1298,59 +1477,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1367,29 +1559,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -1397,59 +1594,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1466,29 +1676,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -1496,59 +1711,72 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="23.0"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1565,29 +1793,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
@@ -1595,8 +1828,7 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>